<commit_message>
Added goal 2 analysis
</commit_message>
<xml_diff>
--- a/PyBullet/timings.xlsx
+++ b/PyBullet/timings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Robot-task-planning\PyBullet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C0DBB2-2B88-456D-AD93-DB58415064DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987CABA4-698F-4036-9330-CB61167A2FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Goal 5" sheetId="1" r:id="rId1"/>
+    <sheet name="Goal 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Goal 5" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="7">
   <si>
     <t>World</t>
   </si>
@@ -362,11 +363,729 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B38F897-D79B-4B11-BE2E-4F1B8D408A12}">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49260.081502045701</v>
+      </c>
+      <c r="C2">
+        <v>70447.732474781893</v>
+      </c>
+      <c r="D2">
+        <v>128596.92701965899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>34887.1846051229</v>
+      </c>
+      <c r="C3">
+        <v>44184.556325680504</v>
+      </c>
+      <c r="D3">
+        <v>55952.754051457203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>43984.346516044803</v>
+      </c>
+      <c r="C4">
+        <v>71461.934882409201</v>
+      </c>
+      <c r="D4">
+        <v>170129.46007863199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>60097.9690427717</v>
+      </c>
+      <c r="C5">
+        <v>217504.94307903</v>
+      </c>
+      <c r="D5">
+        <v>692209.77471155103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>35056.049801858499</v>
+      </c>
+      <c r="C6">
+        <v>41933.495021554503</v>
+      </c>
+      <c r="D6">
+        <v>50785.410507758599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>34952.697042174099</v>
+      </c>
+      <c r="C7">
+        <v>50276.5917783205</v>
+      </c>
+      <c r="D7">
+        <v>62050.285459474202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>44008.751042916803</v>
+      </c>
+      <c r="C8">
+        <v>55034.7844003352</v>
+      </c>
+      <c r="D8">
+        <v>67762.5807125641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>29908.4532416406</v>
+      </c>
+      <c r="C9">
+        <v>52759.893584238402</v>
+      </c>
+      <c r="D9">
+        <v>75567.226973988902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>35091.061916969396</v>
+      </c>
+      <c r="C10">
+        <v>48009.464141524099</v>
+      </c>
+      <c r="D10">
+        <v>63424.394427009698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>34918.595787494101</v>
+      </c>
+      <c r="C11">
+        <v>46168.599362492001</v>
+      </c>
+      <c r="D11">
+        <v>64545.752171613902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>4.375</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5.2857142857142803</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>7.8181818181818103</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4.2857142857142803</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4.5714285714285703</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>6.4166666666666599</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3.8571428571428501</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3.71428571428571</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>31.636363636363601</v>
+      </c>
+      <c r="D24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>19.375</v>
+      </c>
+      <c r="D25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>25.857142857142801</v>
+      </c>
+      <c r="D26">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>18.285714285714199</v>
+      </c>
+      <c r="D28">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>22.857142857142801</v>
+      </c>
+      <c r="D30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>26.1666666666666</v>
+      </c>
+      <c r="D31">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>20.428571428571399</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>19.571428571428498</v>
+      </c>
+      <c r="D33">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EF09C6D3-0756-4013-B3F3-F3744A26A740}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B21">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0536ABEA-95C9-4BF4-AD65-2FBE751B6DB1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:B33">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{27C92049-F005-427E-B019-B8C1F771ABA7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8C2279BE-BE89-477A-9767-599DBEFE6FA7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C22">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CF76091E-AE65-42E6-A469-D9FA25E03D80}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:C33">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4DA91F7E-48C7-4436-96C5-8C3F9C826171}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{75ADB481-B4AB-49D8-B4B6-10EFF9B3849F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D22">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{40127D5F-B78E-4B0F-A58C-D6826FF017A5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D33">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7286D1A6-9922-465B-992A-747375BFAC3F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EF09C6D3-0756-4013-B3F3-F3744A26A740}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B2:B11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0536ABEA-95C9-4BF4-AD65-2FBE751B6DB1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B13:B21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{27C92049-F005-427E-B019-B8C1F771ABA7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B24:B33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8C2279BE-BE89-477A-9767-599DBEFE6FA7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C2:C11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CF76091E-AE65-42E6-A469-D9FA25E03D80}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C13:C22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4DA91F7E-48C7-4436-96C5-8C3F9C826171}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C24:C33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{75ADB481-B4AB-49D8-B4B6-10EFF9B3849F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:D11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{40127D5F-B78E-4B0F-A58C-D6826FF017A5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D13:D22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7286D1A6-9922-465B-992A-747375BFAC3F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D24:D33</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I40" sqref="A1:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>